<commit_message>
Fix typo in CC1101_Frequenz calculation sheet
</commit_message>
<xml_diff>
--- a/Info/CC1101_Frequenz/CC1101_Frequenz.xlsx
+++ b/Info/CC1101_Frequenz/CC1101_Frequenz.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>MHz</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>75 kHz höher</t>
+  </si>
+  <si>
+    <t>FREQ[23:0] hex</t>
   </si>
 </sst>
 </file>
@@ -535,7 +538,7 @@
   <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update CC1101 frequency calc excel sheet
</commit_message>
<xml_diff>
--- a/Info/CC1101_Frequenz/CC1101_Frequenz.xlsx
+++ b/Info/CC1101_Frequenz/CC1101_Frequenz.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>MHz</t>
   </si>
@@ -32,16 +32,27 @@
   </si>
   <si>
     <t>FREQ[23:0] hex</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Dez</t>
+  </si>
+  <si>
+    <t>Frequenz MHz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,13 +68,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -87,7 +110,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -535,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D6"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +591,7 @@
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="6">
         <v>868.29986599999995</v>
       </c>
       <c r="B4" s="1">
@@ -609,6 +636,32 @@
       </c>
       <c r="D6" s="3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="5">
+        <v>216562</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <f>HEX2DEC(B19)</f>
+        <v>2188642</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="4">
+        <f>B20*26/65536</f>
+        <v>868.29669189453125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>